<commit_message>
Solved binary/bit manipulation 21 Jan 2021
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DC4AE3-4C12-47BB-BCCA-D68DC0C006F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5C6B42-FB02-478F-825E-193AA8667248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,9 +178,6 @@
     <t>https://leetcode.com/problems/sum-of-two-integers/</t>
   </si>
   <si>
-    <t>add bit by bit, be mindful of carry, after adding, if carry is still 1, then add it as well;</t>
-  </si>
-  <si>
     <t>https://youtu.be/5Km3utixwZs</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>https://leetcode.com/problems/counting-bits/</t>
   </si>
   <si>
-    <t>write out result for num=16 to figure out pattern; res[i] = res[i - offset], where offset is the biggest power of 2 &lt;= I;</t>
-  </si>
-  <si>
     <t>https://youtu.be/WnPLSRLSANE</t>
   </si>
   <si>
@@ -992,13 +986,19 @@
   </si>
   <si>
     <t>Stats</t>
+  </si>
+  <si>
+    <t>add bit by bit, be mindful of carry, after adding, if carry is still 1, then add it as well; python mask the number with 0xffffffff ref sol</t>
+  </si>
+  <si>
+    <t>ref number of 1s in optimal solution in prev question and do for all numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1024,11 +1024,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1112,21 +1107,40 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1176,8 +1190,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1229,77 +1271,87 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="14" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1324,23 +1376,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1711,7 +1763,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FB6FD29-B17D-455D-A3D6-0D514F3753B0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1778,7 +1830,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02947540-B2C2-4AB6-9E8C-2E3895083E69}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1845,7 +1897,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541D7459-65E2-4FC6-BAAD-8651374B89AB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1912,7 +1964,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF83A75-6975-46B3-AC37-E20A6BC35C31}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1979,7 +2031,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62FBB29E-A352-48E7-90F5-210E8485C915}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2046,7 +2098,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D53F4C9-0D2F-4B0B-8324-4F1CEAEC8DC8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2113,7 +2165,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{254FE3BD-0A57-4CB1-8518-D9CC6825C31C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2180,7 +2232,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC0102B-974C-49E1-A0E2-595ACFFBDFC5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2247,7 +2299,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D493AB9D-1AC7-4458-A852-903002A666FA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2314,7 +2366,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10FBEC2D-C98C-474A-9848-C2FFEC8D99BA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2381,7 +2433,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA196EDF-DA16-47C3-B840-18F96D1D3D6D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2448,7 +2500,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC426C1E-4280-4278-B643-1DDD270A9D9E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2515,7 +2567,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BE85AA-2D0C-4EC3-BB00-5A489189C7B6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2582,7 +2634,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{584DBCC3-DEF8-4ECD-ADB5-C7FD11B36B0D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2649,7 +2701,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5127C57A-E6E5-4903-BDCB-52608B832FCF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2716,7 +2768,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85E9C481-3DDF-4769-8242-CAA870246E20}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2783,7 +2835,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BC6F07-D7A4-43A5-A39E-F5016CB04E38}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2850,7 +2902,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E234E640-D19A-44BC-9371-A61A4B135AFE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2917,7 +2969,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{202BEDB4-306E-4941-91C5-51D97FD3C450}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2984,7 +3036,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3829CD-62D8-4826-BF8C-3D097DA05CA8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3051,7 +3103,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07439E9D-65B6-4909-8048-563084F7A964}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3118,7 +3170,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B6790CD-CC63-4B9D-B787-5ECACE2B2CD5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3185,7 +3237,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362604DB-92A7-4576-B858-81FFAB8FC0FB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3252,7 +3304,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8816BF94-6849-4F55-9B27-3A46FA977496}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3319,7 +3371,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1CF4FC3-9B42-4520-8D76-8A630BC3ADF5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3386,7 +3438,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{033EABBE-906E-4149-AC68-9AF492BBA8FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3453,7 +3505,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{635BE2DC-B4B1-4C74-A161-9552222A8495}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3520,7 +3572,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11BC6735-43F1-42AC-A585-BEC73F599912}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3587,7 +3639,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7351C912-E875-495A-99D5-748F95DAE8C5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3654,7 +3706,7 @@
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{185E5FC8-7130-404B-9DCF-7FE579E8EE52}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3721,7 +3773,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28555DD-5338-4BBB-AA94-6D6454D6AA2B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3788,7 +3840,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62CE5628-A09B-4396-9A45-817CEE3BEB87}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3855,7 +3907,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A5BB2D-80CA-4AE4-94FD-407F8A4001E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3922,7 +3974,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BECBE65-73F2-40DF-A213-537CFB0204C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3989,7 +4041,7 @@
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4765664-4FF7-4870-9A31-C59FBBFB3879}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4056,7 +4108,7 @@
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFC26ABD-7015-48C1-840D-1B48C3400351}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4123,7 +4175,7 @@
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7DF126-937A-4ACA-B52D-BA0CB06F8246}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4190,7 +4242,7 @@
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{351447D8-3747-4965-90A1-073C9D669543}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4257,7 +4309,7 @@
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94BBC97F-6A67-420C-A930-A57A9A0D0171}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4324,7 +4376,7 @@
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3831864-2BB4-4604-A176-BEA886930FFB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4391,7 +4443,7 @@
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B85960F4-ECE1-4990-9631-3B187A9F12A1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4458,7 +4510,7 @@
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8E3F3D7-DE0C-492E-AA4F-C9B4DDB6E735}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4525,7 +4577,7 @@
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F31D20-E021-41E9-A1D7-50371E8B7245}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4592,7 +4644,7 @@
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C15A25F0-2C94-4001-9FEB-05628544D408}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4659,7 +4711,7 @@
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{583DFC1B-E2D9-49CD-B386-6A8C290DDE43}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4726,7 +4778,7 @@
                   <a14:compatExt spid="_x0000_s1074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC2F58C6-1738-4AD2-9541-9010D7000F83}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4793,7 +4845,7 @@
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84755B7-6B69-403D-BD90-533D074B6A5B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4860,7 +4912,7 @@
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA4C118-EAF8-4AC4-93B6-E4C8CA5064FA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4927,7 +4979,7 @@
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52D6FE80-2BCD-471B-BD90-28E0C3FD915F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4994,7 +5046,7 @@
                   <a14:compatExt spid="_x0000_s1078"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5343094-D804-4230-BA2F-4C87C213E772}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5061,7 +5113,7 @@
                   <a14:compatExt spid="_x0000_s1079"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C7B9A5-76C3-405D-82C5-4BF3B6EA75C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5128,7 +5180,7 @@
                   <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{364389B6-6139-490F-A50C-FC3389A763DE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5195,7 +5247,7 @@
                   <a14:compatExt spid="_x0000_s1081"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFE130CF-590B-4AAC-9E85-C719DB1B3D00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5262,7 +5314,7 @@
                   <a14:compatExt spid="_x0000_s1082"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CFD3F4E-EBAD-4572-A352-034186AC9F96}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5329,7 +5381,7 @@
                   <a14:compatExt spid="_x0000_s1083"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45CDC75C-F87F-41DC-8B88-7C4AF875FAC2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5396,7 +5448,7 @@
                   <a14:compatExt spid="_x0000_s1084"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{151F0C3D-71AC-4853-94E9-7B42FA5F4332}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5463,7 +5515,7 @@
                   <a14:compatExt spid="_x0000_s1085"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C80B2FA0-9854-46DA-83FE-E9E6AF9B9F58}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5530,7 +5582,7 @@
                   <a14:compatExt spid="_x0000_s1086"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D64C1ACA-562C-4BF9-8D13-B40E93D4322E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5597,7 +5649,7 @@
                   <a14:compatExt spid="_x0000_s1087"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5270E61-C854-4D45-B052-62BDD1E0D049}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5664,7 +5716,7 @@
                   <a14:compatExt spid="_x0000_s1088"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B9D234B-B840-401B-80C8-25FC62273B88}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5731,7 +5783,7 @@
                   <a14:compatExt spid="_x0000_s1089"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEFEE4EF-F2E7-4202-9418-4D575FD41CFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5798,7 +5850,7 @@
                   <a14:compatExt spid="_x0000_s1090"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D2FCD48-313B-4657-A121-4F04B93C256B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5865,7 +5917,7 @@
                   <a14:compatExt spid="_x0000_s1091"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59D7459-2008-4441-8928-F21D624D5CA6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5932,7 +5984,7 @@
                   <a14:compatExt spid="_x0000_s1092"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7894197-2271-4B34-AFEF-8EB36A9BA2E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5999,7 +6051,7 @@
                   <a14:compatExt spid="_x0000_s1093"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{858F270D-5839-4C3B-8A4D-9C3682505EFE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6066,7 +6118,7 @@
                   <a14:compatExt spid="_x0000_s1094"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAB89455-E6FD-4E76-ADAB-22B8955F1CBF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6133,7 +6185,7 @@
                   <a14:compatExt spid="_x0000_s1095"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA64EFB-1E01-4A7B-9C09-943E2ACFC9EC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6200,7 +6252,7 @@
                   <a14:compatExt spid="_x0000_s1096"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B57C4B-CDC8-4505-B4B8-40B565131D70}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6267,7 +6319,7 @@
                   <a14:compatExt spid="_x0000_s1097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8649F988-90EE-4252-82CC-A107DED6C4AE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6334,7 +6386,7 @@
                   <a14:compatExt spid="_x0000_s1098"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CDB9A1B-C31B-4908-85AA-9DABD8F85B97}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6401,7 +6453,7 @@
                   <a14:compatExt spid="_x0000_s1099"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84519E92-7F55-45C1-AAD4-6F5B4E2D9766}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6468,7 +6520,7 @@
                   <a14:compatExt spid="_x0000_s1100"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C667E65E-09CE-4E41-88B4-737350B83B39}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6535,7 +6587,7 @@
                   <a14:compatExt spid="_x0000_s1101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{911BD74A-BDF0-4611-BC55-7B7F07901CE3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6602,7 +6654,7 @@
                   <a14:compatExt spid="_x0000_s1102"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F1FCC8C-486C-4687-A3AC-BED5C5A8B27D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6669,7 +6721,7 @@
                   <a14:compatExt spid="_x0000_s1103"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D41E95A-E85B-409E-B5DB-89BFCE6D671E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6920,7 +6972,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6937,1484 +6989,1484 @@
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="F1" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="15"/>
+      <c r="F2" s="9"/>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="I2" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="J2" s="21">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="9"/>
       <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="I3" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="J3" s="21">
         <f>COUNTIF(G2:G77, TRUE)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="J4" s="7">
+      <c r="I4" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="J4" s="22">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.21052631578947367</v>
+        <v>0.27631578947368424</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="9"/>
       <c r="G5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="9"/>
       <c r="G6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="9"/>
       <c r="G7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="9"/>
       <c r="G8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="9"/>
       <c r="G9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="9"/>
       <c r="G10" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="9"/>
       <c r="G11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="D13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="D14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="C15" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="E15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="14" t="s">
+      <c r="C16" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="E16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="B17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="C17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="E17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="9"/>
       <c r="G17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="16" t="s">
+      <c r="E18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="D19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="16" t="s">
+      <c r="E19" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="16" t="s">
+      <c r="E20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="B21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="D21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="16" t="s">
+      <c r="E21" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="B22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="16" t="s">
+      <c r="E22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="B23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="D23" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="E23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="B24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="D24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="16" t="s">
+      <c r="E24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="B25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="D25" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="16" t="s">
+      <c r="E25" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="B26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="D26" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="16" t="s">
+      <c r="E26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="B27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="D27" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="16" t="s">
+      <c r="E27" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="B28" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="C28" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="D28" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="E28" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="B29" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="D29" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="16" t="s">
+      <c r="E29" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="B30" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="D30" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="16" t="s">
+      <c r="E30" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="B31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="D31" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="16" t="s">
+      <c r="E31" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="B32" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+      <c r="D32" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="18" t="s">
+      <c r="E32" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="B33" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="F32" s="15"/>
-    </row>
-    <row r="33" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="D33" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="18" t="s">
+      <c r="E33" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="B34" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="D34" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B34" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="16" t="s">
+      <c r="E34" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="B35" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="D35" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="16" t="s">
+      <c r="E35" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="B36" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+      <c r="C36" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="D36" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="E36" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="B37" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="F36" s="15"/>
-    </row>
-    <row r="37" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="D37" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="16" t="s">
+      <c r="E37" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="B38" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="F37" s="15"/>
-    </row>
-    <row r="38" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="D38" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C38" s="16" t="s">
+      <c r="E38" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="B39" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F38" s="15"/>
-    </row>
-    <row r="39" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+      <c r="D39" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B39" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="E39" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="B40" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21" t="s">
+      <c r="D40" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B40" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="16" t="s">
+      <c r="E40" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="B41" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F40" s="15"/>
-    </row>
-    <row r="41" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
+      <c r="C41" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="D41" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="E41" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="F41" s="15"/>
+      <c r="F41" s="9"/>
       <c r="G41" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="12" t="s">
+      <c r="E42" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="F42" s="15"/>
+      <c r="F42" s="9"/>
       <c r="G42" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C43" s="12" t="s">
+      <c r="E43" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="F43" s="15"/>
+      <c r="F43" s="9"/>
       <c r="G43" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44" s="18" t="s">
+      <c r="E44" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="F44" s="15"/>
+      <c r="F44" s="9"/>
       <c r="G44" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C45" s="16" t="s">
+      <c r="E45" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="F45" s="15"/>
+      <c r="F45" s="9"/>
       <c r="G45" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C46" s="16" t="s">
+      <c r="E46" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" s="15"/>
+      <c r="F46" s="9"/>
       <c r="G46" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="D47" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="E47" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="B48" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F47" s="15"/>
-    </row>
-    <row r="48" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
+      <c r="D48" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="16" t="s">
+      <c r="E48" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="B49" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="F48" s="15"/>
-    </row>
-    <row r="49" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="D49" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="C49" s="16" t="s">
+      <c r="E49" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="B50" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F49" s="15"/>
-    </row>
-    <row r="50" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
+      <c r="D50" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="C50" s="16" t="s">
+      <c r="E50" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="B51" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F50" s="15"/>
-    </row>
-    <row r="51" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="D51" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="E51" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="B52" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="F51" s="15"/>
-    </row>
-    <row r="52" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
+      <c r="D52" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C52" s="16" t="s">
+      <c r="E52" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="B53" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="F52" s="15"/>
-    </row>
-    <row r="53" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="22" t="s">
+      <c r="D53" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B53" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C53" s="18" t="s">
+      <c r="E53" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="B54" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="F53" s="15"/>
-    </row>
-    <row r="54" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="10" t="s">
+      <c r="D54" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C54" s="12" t="s">
+      <c r="E54" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="B55" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="F54" s="15"/>
-    </row>
-    <row r="55" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
+      <c r="D55" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B55" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C55" s="16" t="s">
+      <c r="E55" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="B56" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F55" s="15"/>
-    </row>
-    <row r="56" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+      <c r="D56" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B56" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C56" s="12" t="s">
+      <c r="E56" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="B57" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="F56" s="15"/>
-    </row>
-    <row r="57" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
+      <c r="D57" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C57" s="12" t="s">
+      <c r="E57" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="B58" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="F57" s="15"/>
-    </row>
-    <row r="58" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="D58" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C58" s="16" t="s">
+      <c r="E58" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="B59" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="F58" s="15"/>
-    </row>
-    <row r="59" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="10" t="s">
+      <c r="D59" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C59" s="16" t="s">
+      <c r="E59" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="B60" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="F59" s="15"/>
-    </row>
-    <row r="60" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="19" t="s">
+      <c r="D60" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B60" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="C60" s="16" t="s">
+      <c r="E60" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="B61" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="F60" s="15"/>
-    </row>
-    <row r="61" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="10" t="s">
+      <c r="C61" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="D61" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="E61" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="B62" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="F61" s="15"/>
-    </row>
-    <row r="62" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="10" t="s">
+      <c r="D62" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C62" s="12" t="s">
+      <c r="E62" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="B63" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="F62" s="15"/>
-    </row>
-    <row r="63" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="10" t="s">
+      <c r="D63" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C63" s="12" t="s">
+      <c r="E63" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="B64" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="F63" s="15"/>
-    </row>
-    <row r="64" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
+      <c r="D64" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C64" s="18" t="s">
+      <c r="E64" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="F64" s="9"/>
+    </row>
+    <row r="65" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="B65" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="F64" s="15"/>
-    </row>
-    <row r="65" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="10" t="s">
+      <c r="D65" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="B65" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C65" s="16" t="s">
+      <c r="E65" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="F65" s="9"/>
+    </row>
+    <row r="66" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="B66" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F65" s="15"/>
-    </row>
-    <row r="66" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
+      <c r="D66" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C66" s="18" t="s">
+      <c r="E66" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="B67" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="F66" s="15"/>
-    </row>
-    <row r="67" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="10" t="s">
+      <c r="D67" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C67" s="12" t="s">
+      <c r="E67" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="B68" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="F67" s="15"/>
-    </row>
-    <row r="68" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
+      <c r="D68" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C68" s="16" t="s">
+      <c r="E68" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="D68" s="13" t="s">
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E68" s="14" t="s">
+      <c r="B69" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="F68" s="15"/>
-    </row>
-    <row r="69" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
+      <c r="D69" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C69" s="16" t="s">
+      <c r="E69" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="F69" s="9"/>
+    </row>
+    <row r="70" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="B70" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="F69" s="15"/>
-    </row>
-    <row r="70" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
+      <c r="D70" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C70" s="16" t="s">
+      <c r="E70" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="F70" s="9"/>
+    </row>
+    <row r="71" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="B71" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="F70" s="15"/>
-    </row>
-    <row r="71" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
+      <c r="D71" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C71" s="12" t="s">
+      <c r="E71" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="B72" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C72" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="F71" s="15"/>
-    </row>
-    <row r="72" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
+      <c r="D72" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C72" s="16" t="s">
+      <c r="E72" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="F72" s="9"/>
+    </row>
+    <row r="73" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="B73" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="F72" s="15"/>
-    </row>
-    <row r="73" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
+      <c r="D73" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C73" s="16" t="s">
+      <c r="E73" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="B74" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C74" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="F73" s="15"/>
-    </row>
-    <row r="74" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
+      <c r="D74" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C74" s="18" t="s">
+      <c r="E74" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="F74" s="9"/>
+    </row>
+    <row r="75" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="E74" s="14" t="s">
+      <c r="C75" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E75" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="F74" s="15"/>
-    </row>
-    <row r="75" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B75" s="11" t="s">
+      <c r="F75" s="9"/>
+    </row>
+    <row r="76" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C75" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E75" s="14" t="s">
+      <c r="B76" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C76" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F75" s="15"/>
-    </row>
-    <row r="76" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="10" t="s">
+      <c r="D76" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="B76" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="C76" s="16" t="s">
+      <c r="E76" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="E76" s="14" t="s">
+      <c r="B77" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C77" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="F76" s="15"/>
-    </row>
-    <row r="77" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="10" t="s">
+      <c r="D77" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="B77" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="C77" s="18" t="s">
+      <c r="E77" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="D77" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="E77" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="F77" s="15"/>
+      <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>

</xml_diff>

<commit_message>
Partial completion of graphs
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5C6B42-FB02-478F-825E-193AA8667248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF2B8B1-22C1-4ACB-B446-37AC68FE36E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>https://leetcode.com/problems/maximum-subarray/</t>
   </si>
   <si>
-    <t>pattern: prev subarray cant be negative, dynamic programming: compute max sum for each prefix</t>
-  </si>
-  <si>
     <t>https://youtu.be/lXVy6YWFcRM</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>https://youtu.be/Y0lT9Fck7qI</t>
   </si>
   <si>
-    <t>Dynamic Programming</t>
-  </si>
-  <si>
     <t>Climbing Stairs</t>
   </si>
   <si>
@@ -451,12 +445,6 @@
     <t>Number of Connected Components in an Undirected Graph (Leetcode Premium)</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/</t>
-  </si>
-  <si>
-    <t>dfs on each node that hasn’t been visited, increment component count, adjacency list; bfs and union find are possible;</t>
-  </si>
-  <si>
     <t>https://youtu.be/A8NUOmlwOlM</t>
   </si>
   <si>
@@ -992,13 +980,25 @@
   </si>
   <si>
     <t>ref number of 1s in optimal solution in prev question and do for all numbers</t>
+  </si>
+  <si>
+    <t>pattern: prev subarray cant be negative, DP: compute max sum for each prefix</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-provinces/submissions/</t>
+  </si>
+  <si>
+    <t>dfs on each node that hasn’t been visited, increment component count, adjacency list; bfs and union find are possible; original link (https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1139,6 +1139,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1271,14 +1283,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1328,12 +1341,6 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="14" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1346,10 +1353,20 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,15 +1417,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1416,43 +1433,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1460,11 +1477,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1476,7 +1493,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1560,23 +1577,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$54" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$55" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$56" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$57" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$58" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1592,19 +1609,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$61" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1636,7 +1653,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$71" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1660,7 +1677,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1683,8 +1700,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1750,8 +1767,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1817,8 +1834,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1884,8 +1901,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1951,8 +1968,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2018,8 +2035,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2085,8 +2102,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2152,8 +2169,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2219,8 +2236,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2286,8 +2303,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2353,8 +2370,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2420,8 +2437,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2487,8 +2504,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2554,8 +2571,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2621,8 +2638,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2688,8 +2705,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2755,8 +2772,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2822,8 +2839,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2889,8 +2906,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2956,8 +2973,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3023,8 +3040,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3090,8 +3107,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3157,8 +3174,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3224,8 +3241,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3291,8 +3308,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3358,8 +3375,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3425,8 +3442,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3492,8 +3509,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3559,8 +3576,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3626,8 +3643,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3693,8 +3710,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3760,8 +3777,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3827,8 +3844,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3894,8 +3911,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3961,8 +3978,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4028,8 +4045,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4095,8 +4112,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4162,8 +4179,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4229,8 +4246,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>39</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4296,8 +4313,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4363,8 +4380,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4430,8 +4447,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>42</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4497,8 +4514,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4564,8 +4581,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>44</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4631,8 +4648,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>45</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4698,8 +4715,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>46</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4765,8 +4782,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>47</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4832,8 +4849,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4899,8 +4916,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>49</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4966,8 +4983,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>50</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5033,8 +5050,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>51</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5100,8 +5117,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>52</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5167,8 +5184,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>53</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5234,8 +5251,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>54</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5301,8 +5318,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>55</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5368,8 +5385,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>56</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5435,8 +5452,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>57</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5502,8 +5519,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>58</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5569,8 +5586,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>59</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5636,8 +5653,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>60</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5703,8 +5720,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>61</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5770,8 +5787,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>62</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5837,8 +5854,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>64</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5904,8 +5921,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>63</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5971,8 +5988,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>65</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6038,8 +6055,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>66</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6105,8 +6122,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>67</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6172,8 +6189,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>68</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6239,8 +6256,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6306,8 +6323,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>70</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6373,8 +6390,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>71</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6440,8 +6457,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>72</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6507,8 +6524,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>73</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6574,8 +6591,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>74</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6641,8 +6658,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>75</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6708,8 +6725,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
           <xdr:row>76</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6971,27 +6988,27 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="100.140625" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
@@ -7006,12 +7023,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="J1" s="20"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -7033,10 +7050,10 @@
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="21" t="s">
-        <v>315</v>
-      </c>
-      <c r="J2" s="21">
+      <c r="I2" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="J2" s="19">
         <v>76</v>
       </c>
     </row>
@@ -7060,12 +7077,12 @@
       <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="J3" s="21">
+      <c r="I3" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="J3" s="19">
         <f>COUNTIF(G2:G77, TRUE)</f>
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7089,12 +7106,12 @@
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="J4" s="22">
+      <c r="I4" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="J4" s="20">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.27631578947368424</v>
+        <v>0.35526315789473684</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7132,7 +7149,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>24</v>
+        <v>317</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" t="b">
@@ -7141,19 +7158,19 @@
     </row>
     <row r="7" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" t="b">
@@ -7162,19 +7179,19 @@
     </row>
     <row r="8" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" t="b">
@@ -7183,19 +7200,19 @@
     </row>
     <row r="9" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" t="b">
@@ -7204,19 +7221,19 @@
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" t="b">
@@ -7225,19 +7242,19 @@
     </row>
     <row r="11" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" t="b">
@@ -7246,19 +7263,19 @@
     </row>
     <row r="12" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="D12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="E12" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" t="b">
@@ -7267,19 +7284,19 @@
     </row>
     <row r="13" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" t="b">
@@ -7288,19 +7305,19 @@
     </row>
     <row r="14" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>55</v>
-      </c>
       <c r="E14" s="8" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" t="b">
@@ -7309,19 +7326,19 @@
     </row>
     <row r="15" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" t="b">
@@ -7330,19 +7347,19 @@
     </row>
     <row r="16" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="23" t="s">
+      <c r="D16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" t="b">
@@ -7351,19 +7368,19 @@
     </row>
     <row r="17" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="D17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E17" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" t="b">
@@ -7372,433 +7389,481 @@
     </row>
     <row r="18" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="F18" s="9"/>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="F19" s="9"/>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="F20" s="9"/>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="F21" s="9"/>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="F22" s="9"/>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="F23" s="9"/>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>96</v>
-      </c>
       <c r="F24" s="9"/>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="F25" s="9"/>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="E26" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="F26" s="9"/>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="F27" s="9"/>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="D28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="F28" s="9"/>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="E29" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="F29" s="9"/>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="10" t="s">
+      <c r="E30" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="F30" s="9"/>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="E31" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="F31" s="9"/>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="12" t="s">
+      <c r="E32" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="F32" s="9"/>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="12" t="s">
+      <c r="E33" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>133</v>
       </c>
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="10" t="s">
+      <c r="E34" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>319</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>141</v>
+        <v>320</v>
       </c>
       <c r="F35" s="9"/>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" t="b">
@@ -7807,19 +7872,19 @@
     </row>
     <row r="42" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" t="b">
@@ -7828,19 +7893,19 @@
     </row>
     <row r="43" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" t="b">
@@ -7849,19 +7914,19 @@
     </row>
     <row r="44" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" t="b">
@@ -7870,19 +7935,19 @@
     </row>
     <row r="45" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" t="b">
@@ -7891,19 +7956,19 @@
     </row>
     <row r="46" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" t="b">
@@ -7912,569 +7977,599 @@
     </row>
     <row r="47" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C48" s="10" t="s">
+      <c r="B49" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C49" s="10" t="s">
+      <c r="B50" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D50" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C50" s="10" t="s">
+      <c r="B51" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="C51" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="E51" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="B52" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" s="10" t="s">
+      <c r="B53" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E53" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="F52" s="9"/>
-    </row>
-    <row r="53" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C53" s="12" t="s">
+      <c r="B54" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D54" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="F53" s="9"/>
-    </row>
-    <row r="54" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="F54" s="9"/>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C54" s="6" t="s">
+      <c r="B55" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E55" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="F55" s="9"/>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C55" s="10" t="s">
+      <c r="B56" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="F55" s="9"/>
-    </row>
-    <row r="56" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="F56" s="9"/>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C56" s="6" t="s">
+      <c r="B57" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E57" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="F56" s="9"/>
-    </row>
-    <row r="57" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="F57" s="9"/>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="B58" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D58" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E58" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="F57" s="9"/>
-    </row>
-    <row r="58" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="F58" s="9"/>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C58" s="10" t="s">
+      <c r="B59" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D59" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="F58" s="9"/>
-    </row>
-    <row r="59" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C59" s="10" t="s">
+      <c r="B60" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D60" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="F59" s="9"/>
-    </row>
-    <row r="60" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B60" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="C60" s="10" t="s">
+      <c r="B61" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="D61" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="F60" s="9"/>
-    </row>
-    <row r="61" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="E61" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="F61" s="9"/>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="B62" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D62" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E62" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="62" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="F62" s="9"/>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C62" s="6" t="s">
+      <c r="B63" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="F63" s="9"/>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C63" s="6" t="s">
+      <c r="B64" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C64" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D64" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="F63" s="9"/>
-    </row>
-    <row r="64" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="F64" s="9"/>
+    </row>
+    <row r="65" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C64" s="12" t="s">
+      <c r="B65" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="F64" s="9"/>
-    </row>
-    <row r="65" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="F65" s="9"/>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C65" s="10" t="s">
+      <c r="B66" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D66" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="F65" s="9"/>
-    </row>
-    <row r="66" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C66" s="12" t="s">
+      <c r="B67" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D67" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="F66" s="9"/>
-    </row>
-    <row r="67" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C67" s="6" t="s">
+      <c r="B68" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D68" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F67" s="9"/>
-    </row>
-    <row r="68" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C68" s="10" t="s">
+      <c r="B69" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D69" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="F68" s="9"/>
-    </row>
-    <row r="69" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="F69" s="9"/>
+    </row>
+    <row r="70" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C69" s="10" t="s">
+      <c r="B70" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D70" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="F69" s="9"/>
-    </row>
-    <row r="70" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="F70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C70" s="10" t="s">
+      <c r="B71" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="F70" s="9"/>
-    </row>
-    <row r="71" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="F71" s="9"/>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C71" s="6" t="s">
+      <c r="B72" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C72" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D72" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="F72" s="9"/>
+    </row>
+    <row r="73" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C72" s="10" t="s">
+      <c r="B73" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D73" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E73" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="F72" s="9"/>
-    </row>
-    <row r="73" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C73" s="10" t="s">
+      <c r="B74" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C74" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D74" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E74" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="F73" s="9"/>
-    </row>
-    <row r="74" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="F74" s="9"/>
+    </row>
+    <row r="75" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C74" s="12" t="s">
+      <c r="C75" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E75" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="F75" s="9"/>
+    </row>
+    <row r="76" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="B76" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C76" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="F74" s="9"/>
-    </row>
-    <row r="75" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B75" s="5" t="s">
+      <c r="D76" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E75" s="8" t="s">
+      <c r="E76" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="F75" s="9"/>
-    </row>
-    <row r="76" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="C76" s="10" t="s">
+      <c r="B77" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C77" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D77" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E77" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="F76" s="9"/>
-    </row>
-    <row r="77" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>312</v>
-      </c>
       <c r="F77" s="9"/>
     </row>
-    <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -11414,8 +11509,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11436,8 +11531,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11458,8 +11553,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11480,8 +11575,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11502,8 +11597,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11524,8 +11619,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11546,8 +11641,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11568,8 +11663,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11590,8 +11685,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11612,8 +11707,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11634,8 +11729,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11656,8 +11751,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11678,8 +11773,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11700,8 +11795,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11722,8 +11817,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11744,8 +11839,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>16</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11766,8 +11861,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11788,8 +11883,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11810,8 +11905,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11832,8 +11927,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11854,8 +11949,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11876,8 +11971,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11898,8 +11993,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11920,8 +12015,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11942,8 +12037,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>25</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11964,8 +12059,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11986,8 +12081,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12008,8 +12103,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12030,8 +12125,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12052,8 +12147,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12074,8 +12169,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12096,8 +12191,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12118,8 +12213,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12140,8 +12235,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>34</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12162,8 +12257,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12184,8 +12279,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12206,8 +12301,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12228,8 +12323,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12250,8 +12345,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>39</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12272,8 +12367,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>40</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12294,8 +12389,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>41</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12316,8 +12411,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>42</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12338,8 +12433,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>43</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12360,8 +12455,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>44</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12382,8 +12477,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>45</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12404,8 +12499,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>46</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12426,8 +12521,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>47</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12448,8 +12543,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>48</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12470,8 +12565,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>49</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12492,8 +12587,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>50</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12514,8 +12609,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>51</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12536,8 +12631,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>52</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12558,8 +12653,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>53</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12580,8 +12675,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>54</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12602,8 +12697,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>55</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12624,8 +12719,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>56</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12646,8 +12741,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>57</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12668,8 +12763,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>58</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12690,8 +12785,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>59</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12712,8 +12807,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>60</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12734,8 +12829,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>61</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12756,8 +12851,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>62</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12778,8 +12873,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>64</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12800,8 +12895,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>63</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12822,8 +12917,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>65</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12844,8 +12939,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>66</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12866,8 +12961,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>67</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12888,8 +12983,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>68</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12910,8 +13005,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>69</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12932,8 +13027,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>70</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12954,8 +13049,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>71</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12976,8 +13071,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>72</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12998,8 +13093,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>73</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13020,8 +13115,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>74</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13042,8 +13137,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>75</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13064,8 +13159,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>76</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
Complated Grpahs Jan 22
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF2B8B1-22C1-4ACB-B446-37AC68FE36E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA8D8B7-7D54-4B40-AB53-FE8536EB6BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1353,14 +1353,14 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1485,11 +1485,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6988,8 +6988,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7025,10 +7025,10 @@
       <c r="F1" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="J1" s="24"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -7082,7 +7082,7 @@
       </c>
       <c r="J3" s="19">
         <f>COUNTIF(G2:G77, TRUE)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="J4" s="20">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.35526315789473684</v>
+        <v>0.38157894736842107</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7719,6 +7719,9 @@
         <v>131</v>
       </c>
       <c r="F33" s="9"/>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
@@ -7737,6 +7740,9 @@
         <v>135</v>
       </c>
       <c r="F34" s="9"/>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
@@ -7748,7 +7754,7 @@
       <c r="C35" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="23" t="s">
         <v>319</v>
       </c>
       <c r="E35" s="8" t="s">

</xml_diff>

<commit_message>
Completed DP 22 Jan 2022
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA8D8B7-7D54-4B40-AB53-FE8536EB6BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE53A37-FB99-428D-993C-978F30DA0544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1413,19 +1413,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1433,31 +1433,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1497,23 +1497,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1597,11 +1597,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$59" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$60" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1625,7 +1625,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1700,8 +1700,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1767,8 +1767,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1834,8 +1834,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1901,8 +1901,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1968,8 +1968,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2035,8 +2035,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2102,8 +2102,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2169,8 +2169,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2236,8 +2236,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2303,8 +2303,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2370,8 +2370,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2437,8 +2437,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2504,8 +2504,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2571,8 +2571,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2638,8 +2638,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2705,8 +2705,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2772,8 +2772,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2839,8 +2839,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2906,8 +2906,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2973,8 +2973,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3040,8 +3040,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3107,8 +3107,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3174,8 +3174,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3241,8 +3241,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3308,8 +3308,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3375,8 +3375,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3442,8 +3442,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3509,8 +3509,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3576,8 +3576,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3643,8 +3643,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3710,8 +3710,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3777,8 +3777,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3844,8 +3844,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3911,8 +3911,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3978,8 +3978,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4045,8 +4045,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4112,8 +4112,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4179,8 +4179,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4246,8 +4246,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>39</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4313,8 +4313,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4380,8 +4380,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4447,8 +4447,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>42</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4514,8 +4514,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4581,8 +4581,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>44</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4648,8 +4648,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>45</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4715,8 +4715,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>46</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4782,8 +4782,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>47</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4849,8 +4849,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4916,8 +4916,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>49</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -4983,8 +4983,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>50</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5050,8 +5050,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>51</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5117,8 +5117,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>52</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5184,8 +5184,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>53</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5251,8 +5251,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>54</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5318,8 +5318,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>55</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5385,8 +5385,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>56</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5452,8 +5452,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>57</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5519,8 +5519,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>58</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5586,8 +5586,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>59</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5653,8 +5653,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>60</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5720,8 +5720,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>61</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5787,8 +5787,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>62</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5854,8 +5854,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>64</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5921,8 +5921,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>63</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -5988,8 +5988,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>65</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6055,8 +6055,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>66</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6122,8 +6122,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>67</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6189,8 +6189,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>68</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6256,8 +6256,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6323,8 +6323,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>70</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6390,8 +6390,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>71</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6457,8 +6457,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>72</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6524,8 +6524,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>73</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6591,8 +6591,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>74</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6658,8 +6658,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>75</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6725,8 +6725,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>76</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -6988,8 +6988,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6999,7 +6999,7 @@
     <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="100.140625" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="J3" s="19">
         <f>COUNTIF(G2:G77, TRUE)</f>
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="J4" s="20">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.38157894736842107</v>
+        <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7384,7 +7384,7 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7405,7 +7405,7 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7426,7 +7426,7 @@
       </c>
       <c r="F19" s="9"/>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7447,7 +7447,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7468,7 +7468,7 @@
       </c>
       <c r="F21" s="9"/>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7489,7 +7489,7 @@
       </c>
       <c r="F22" s="9"/>
       <c r="G22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7510,7 +7510,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7531,7 +7531,7 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7573,7 +7573,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7594,7 +7594,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7782,6 +7782,9 @@
         <v>142</v>
       </c>
       <c r="F36" s="9"/>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
@@ -7800,6 +7803,9 @@
         <v>146</v>
       </c>
       <c r="F37" s="9"/>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
@@ -7818,6 +7824,9 @@
         <v>150</v>
       </c>
       <c r="F38" s="9"/>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
@@ -7836,6 +7845,9 @@
         <v>154</v>
       </c>
       <c r="F39" s="9"/>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
@@ -7854,6 +7866,9 @@
         <v>158</v>
       </c>
       <c r="F40" s="9"/>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
@@ -8229,6 +8244,9 @@
         <v>237</v>
       </c>
       <c r="F59" s="9"/>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
@@ -8247,6 +8265,9 @@
         <v>241</v>
       </c>
       <c r="F60" s="9"/>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
@@ -8328,6 +8349,9 @@
         <v>258</v>
       </c>
       <c r="F64" s="9"/>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
@@ -11515,8 +11539,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11537,8 +11561,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11559,8 +11583,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11581,8 +11605,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11603,8 +11627,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11625,8 +11649,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11647,8 +11671,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11669,8 +11693,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11691,8 +11715,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11713,8 +11737,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11735,8 +11759,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11757,8 +11781,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11779,8 +11803,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11801,8 +11825,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11823,8 +11847,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11845,8 +11869,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>16</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11867,8 +11891,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11889,8 +11913,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11911,8 +11935,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11933,8 +11957,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11955,8 +11979,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11977,8 +12001,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11999,8 +12023,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12021,8 +12045,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12043,8 +12067,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>25</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12065,8 +12089,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12087,8 +12111,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12109,8 +12133,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12131,8 +12155,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12153,8 +12177,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12175,8 +12199,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12197,8 +12221,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12219,8 +12243,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12241,8 +12265,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>34</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12263,8 +12287,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12285,8 +12309,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12307,8 +12331,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12329,8 +12353,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12351,8 +12375,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>39</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12373,8 +12397,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>40</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12395,8 +12419,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>41</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12417,8 +12441,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>42</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12439,8 +12463,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>43</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12461,8 +12485,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>44</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12483,8 +12507,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>45</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12505,8 +12529,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>46</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12527,8 +12551,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>47</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12549,8 +12573,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>48</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12571,8 +12595,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>49</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12593,8 +12617,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>50</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12615,8 +12639,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>51</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12637,8 +12661,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>52</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12659,8 +12683,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>53</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12681,8 +12705,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>54</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12703,8 +12727,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>55</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12725,8 +12749,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>56</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12747,8 +12771,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>57</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12769,8 +12793,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>58</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12791,8 +12815,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>59</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12813,8 +12837,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>60</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12835,8 +12859,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>61</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12857,8 +12881,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>62</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12879,8 +12903,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>64</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12901,8 +12925,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>63</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12923,8 +12947,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>65</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12945,8 +12969,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>66</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12967,8 +12991,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>67</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -12989,8 +13013,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>68</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13011,8 +13035,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>69</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13033,8 +13057,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>70</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13055,8 +13079,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>71</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13077,8 +13101,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>72</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13099,8 +13123,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>73</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13121,8 +13145,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>74</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13143,8 +13167,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>75</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -13165,8 +13189,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>76</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
Completed Intervals 23 Jan 2021
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE53A37-FB99-428D-993C-978F30DA0544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D265BC63-AF70-4943-9FC8-CFD148791EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1497,23 +1497,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$39" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6988,8 +6988,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="J3" s="19">
         <f>COUNTIF(G2:G77, TRUE)</f>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="J4" s="20">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.52631578947368418</v>
+        <v>0.59210526315789469</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7783,7 +7783,7 @@
       </c>
       <c r="F36" s="9"/>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7804,7 +7804,7 @@
       </c>
       <c r="F37" s="9"/>
       <c r="G37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7825,7 +7825,7 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7846,7 +7846,7 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7867,7 +7867,7 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Completed Trees 23 Jan 2021
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D265BC63-AF70-4943-9FC8-CFD148791EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C9314C-A92F-44E1-A72A-99020D9D7BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1545,19 +1545,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$47" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$48" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$49" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$50" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1565,15 +1565,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$51" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$52" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$53" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1609,43 +1609,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$61" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$61" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$66" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$67" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$68" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$69" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$70" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1653,31 +1653,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$71" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$71" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$72" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$73" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$74" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$75" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$76" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$77" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1700,7 +1700,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -1767,7 +1767,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -1834,7 +1834,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -1901,7 +1901,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -1968,7 +1968,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2035,7 +2035,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2102,7 +2102,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2169,7 +2169,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2236,7 +2236,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2303,7 +2303,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2370,7 +2370,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2437,7 +2437,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2504,7 +2504,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2571,7 +2571,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2638,7 +2638,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2705,7 +2705,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2772,7 +2772,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2839,7 +2839,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2906,7 +2906,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -2973,7 +2973,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3040,7 +3040,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3107,7 +3107,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3174,7 +3174,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3241,7 +3241,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3308,7 +3308,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3375,7 +3375,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3442,7 +3442,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3509,7 +3509,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3576,7 +3576,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3643,7 +3643,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3710,7 +3710,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3777,7 +3777,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3844,7 +3844,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3911,7 +3911,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -3978,7 +3978,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4045,7 +4045,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4112,7 +4112,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4179,7 +4179,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4246,7 +4246,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>39</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4313,7 +4313,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4380,7 +4380,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4447,7 +4447,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>42</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4514,7 +4514,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4581,7 +4581,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>44</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4648,7 +4648,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>45</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4715,7 +4715,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>46</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4782,7 +4782,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>47</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4849,7 +4849,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4916,7 +4916,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>49</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -4983,7 +4983,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>50</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5050,7 +5050,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>51</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5117,7 +5117,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>52</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5184,7 +5184,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>53</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5251,7 +5251,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>54</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5318,7 +5318,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>55</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5385,7 +5385,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>56</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5452,7 +5452,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>57</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5519,7 +5519,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>58</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5586,7 +5586,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>59</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5653,7 +5653,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>60</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5720,7 +5720,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>61</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5787,7 +5787,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>62</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5854,7 +5854,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>64</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5921,7 +5921,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>63</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -5988,7 +5988,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>65</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6055,7 +6055,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>66</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6122,7 +6122,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>67</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6189,7 +6189,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>68</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6256,7 +6256,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>69</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6323,7 +6323,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>70</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6390,7 +6390,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>71</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6457,7 +6457,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>72</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6524,7 +6524,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>73</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6591,7 +6591,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>74</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6658,7 +6658,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>75</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6725,7 +6725,7 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>104775</xdr:colOff>
           <xdr:row>76</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
@@ -6988,8 +6988,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7000,7 +7000,7 @@
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="100.140625" customWidth="1"/>
     <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="J3" s="19">
         <f>COUNTIF(G2:G77, TRUE)</f>
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="J4" s="20">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.59210526315789469</v>
+        <v>0.77631578947368418</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8013,6 +8013,9 @@
         <v>188</v>
       </c>
       <c r="F47" s="9"/>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
@@ -8031,6 +8034,9 @@
         <v>192</v>
       </c>
       <c r="F48" s="9"/>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
@@ -8049,6 +8055,9 @@
         <v>196</v>
       </c>
       <c r="F49" s="9"/>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
@@ -8067,6 +8076,9 @@
         <v>200</v>
       </c>
       <c r="F50" s="9"/>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
@@ -8085,6 +8097,9 @@
         <v>205</v>
       </c>
       <c r="F51" s="9"/>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
@@ -8103,6 +8118,9 @@
         <v>209</v>
       </c>
       <c r="F52" s="9"/>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
@@ -8121,6 +8139,9 @@
         <v>213</v>
       </c>
       <c r="F53" s="9"/>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
@@ -8287,7 +8308,7 @@
       </c>
       <c r="F61" s="9"/>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8308,7 +8329,7 @@
       </c>
       <c r="F62" s="9"/>
       <c r="G62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8329,7 +8350,7 @@
       </c>
       <c r="F63" s="9"/>
       <c r="G63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8350,7 +8371,7 @@
       </c>
       <c r="F64" s="9"/>
       <c r="G64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8371,7 +8392,7 @@
       </c>
       <c r="F65" s="9"/>
       <c r="G65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8391,6 +8412,9 @@
         <v>266</v>
       </c>
       <c r="F66" s="9"/>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
@@ -8409,6 +8433,9 @@
         <v>270</v>
       </c>
       <c r="F67" s="9"/>
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
@@ -8427,6 +8454,9 @@
         <v>274</v>
       </c>
       <c r="F68" s="9"/>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
@@ -8445,6 +8475,9 @@
         <v>278</v>
       </c>
       <c r="F69" s="9"/>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
@@ -8463,6 +8496,9 @@
         <v>282</v>
       </c>
       <c r="F70" s="9"/>
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
@@ -8482,7 +8518,7 @@
       </c>
       <c r="F71" s="9"/>
       <c r="G71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8502,6 +8538,9 @@
         <v>290</v>
       </c>
       <c r="F72" s="9"/>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
@@ -8520,6 +8559,9 @@
         <v>294</v>
       </c>
       <c r="F73" s="9"/>
+      <c r="G73" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
@@ -8538,6 +8580,9 @@
         <v>298</v>
       </c>
       <c r="F74" s="9"/>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
@@ -8556,6 +8601,9 @@
         <v>300</v>
       </c>
       <c r="F75" s="9"/>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
@@ -8574,6 +8622,9 @@
         <v>304</v>
       </c>
       <c r="F76" s="9"/>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
@@ -8592,6 +8643,9 @@
         <v>308</v>
       </c>
       <c r="F77" s="9"/>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
@@ -11539,7 +11593,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11561,7 +11615,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11583,7 +11637,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11605,7 +11659,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11627,7 +11681,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11649,7 +11703,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11671,7 +11725,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11693,7 +11747,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11715,7 +11769,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11737,7 +11791,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11759,7 +11813,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11781,7 +11835,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11803,7 +11857,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11825,7 +11879,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11847,7 +11901,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11869,7 +11923,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>16</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11891,7 +11945,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11913,7 +11967,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11935,7 +11989,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11957,7 +12011,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -11979,7 +12033,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12001,7 +12055,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12023,7 +12077,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12045,7 +12099,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12067,7 +12121,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>25</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12089,7 +12143,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12111,7 +12165,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12133,7 +12187,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12155,7 +12209,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12177,7 +12231,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12199,7 +12253,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12221,7 +12275,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12243,7 +12297,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12265,7 +12319,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>34</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12287,7 +12341,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12309,7 +12363,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12331,7 +12385,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12353,7 +12407,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12375,7 +12429,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>39</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12397,7 +12451,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>40</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12419,7 +12473,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>41</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12441,7 +12495,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>42</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12463,7 +12517,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>43</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12485,7 +12539,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>44</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12507,7 +12561,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>45</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12529,7 +12583,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>46</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12551,7 +12605,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>47</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12573,7 +12627,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>48</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12595,7 +12649,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>49</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12617,7 +12671,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>50</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12639,7 +12693,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>51</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12661,7 +12715,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>52</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12683,7 +12737,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>53</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12705,7 +12759,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>54</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12727,7 +12781,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>55</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12749,7 +12803,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>56</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12771,7 +12825,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>57</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12793,7 +12847,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>58</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12815,7 +12869,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>59</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12837,7 +12891,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>60</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12859,7 +12913,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>61</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12881,7 +12935,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>62</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12903,7 +12957,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>64</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12925,7 +12979,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>63</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12947,7 +13001,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>65</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12969,7 +13023,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>66</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -12991,7 +13045,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>67</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13013,7 +13067,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>68</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13035,7 +13089,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>69</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13057,7 +13111,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>70</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13079,7 +13133,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>71</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13101,7 +13155,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>72</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13123,7 +13177,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>73</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13145,7 +13199,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>74</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13167,7 +13221,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>75</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
@@ -13189,7 +13243,7 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>76</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>

</xml_diff>

<commit_message>
Completed Matric 23 Jan 2022
</commit_message>
<xml_diff>
--- a/Leetcode-75.xlsx
+++ b/Leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Blind75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C9314C-A92F-44E1-A72A-99020D9D7BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C9C57-D1E2-4A4F-A866-0CD6C65EEF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1545,19 +1545,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$47" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$47" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$48" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$48" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$49" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$49" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$50" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$50" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6988,8 +6988,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="J3" s="19">
         <f>COUNTIF(G2:G77, TRUE)</f>
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="J4" s="20">
         <f>COUNTIF(G2:G77, TRUE)/J2</f>
-        <v>0.77631578947368418</v>
+        <v>0.82894736842105265</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8014,7 +8014,7 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8035,7 +8035,7 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8056,7 +8056,7 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8077,7 +8077,7 @@
       </c>
       <c r="F50" s="9"/>
       <c r="G50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>